<commit_message>
[fix] paper va thoe db moi
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Paper.xlsx
+++ b/MANAGER/Excel_template/Download/Paper.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -44,6 +44,27 @@
     <t>Số tiền</t>
   </si>
   <si>
+    <t>Tên bài báo</t>
+  </si>
+  <si>
+    <t>Tên tạp chí</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Đoàn Văn Thắng</t>
+  </si>
+  <si>
+    <t>HE130002</t>
+  </si>
+  <si>
+    <t>FPTUHN2</t>
+  </si>
+  <si>
+    <t>0 ₫</t>
+  </si>
+  <si>
     <t>Kieu Quoc Tuan</t>
   </si>
   <si>
@@ -53,85 +74,19 @@
     <t>FGWQN</t>
   </si>
   <si>
-    <t>123.711.000 ₫</t>
-  </si>
-  <si>
-    <t>Nguyen Hong Phuc</t>
-  </si>
-  <si>
-    <t>HE130001</t>
-  </si>
-  <si>
-    <t>FPTUHN2</t>
-  </si>
-  <si>
-    <t>20.000.000 ₫</t>
-  </si>
-  <si>
-    <t>Tran Thi Thuy Nguyen</t>
-  </si>
-  <si>
-    <t>HE130003</t>
-  </si>
-  <si>
-    <t>FPLHCM1</t>
-  </si>
-  <si>
-    <t>36.289.000 ₫</t>
-  </si>
-  <si>
-    <t>Vu Minh Hieu</t>
-  </si>
-  <si>
-    <t>HE130004</t>
-  </si>
-  <si>
-    <t>FPLHCM2</t>
-  </si>
-  <si>
-    <t>Tên bài báo</t>
-  </si>
-  <si>
-    <t>Tên tạp chí</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>enim. Mauris quis turpis vitae purus gravida sagittis. Duis gravida. Praesent eu</t>
-  </si>
-  <si>
-    <t>Ligula Tortor Dictum Corp.</t>
-  </si>
-  <si>
-    <t>1 tác giả, 1 địa chỉ FPTU</t>
-  </si>
-  <si>
-    <t>faucibus lectus, a sollicitudin orci sem eget massa. Suspendisse eleifend. Cras</t>
-  </si>
-  <si>
-    <t>Nam Interdum PC</t>
+    <t>10.000.000 ₫</t>
+  </si>
+  <si>
+    <t>paper 3</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
   <si>
     <t>2 tác giả, 2 địa chỉ FPTU</t>
   </si>
   <si>
-    <t>Donec vitae erat vel pede blandit congue. In scelerisque scelerisque dui. Suspendisse ac metus vitae velit</t>
-  </si>
-  <si>
-    <t>Vehicula Aliquet Libero PC</t>
-  </si>
-  <si>
-    <t>3 tác giả, 3 địa chỉ FPTU</t>
-  </si>
-  <si>
-    <t>5.000.000 ₫</t>
-  </si>
-  <si>
-    <t>báo khoa học</t>
-  </si>
-  <si>
-    <t>NXB Hà Nội</t>
+    <t>paper 4</t>
   </si>
 </sst>
 </file>
@@ -459,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -490,13 +445,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -504,22 +459,67 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="3">
+      <c r="E3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>25</v>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -561,127 +561,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="E3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>2</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="E6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>4</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +578,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -727,16 +613,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +650,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
@@ -778,74 +681,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[fix] upload qd paper
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Paper.xlsx
+++ b/MANAGER/Excel_template/Download/Paper.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>STT</t>
   </si>
@@ -44,16 +44,25 @@
     <t>Số tiền</t>
   </si>
   <si>
-    <t>Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>fe001</t>
-  </si>
-  <si>
-    <t>FPTUHN1</t>
-  </si>
-  <si>
-    <t>10.000.000 ₫</t>
+    <t>Kieu Quoc Tuan</t>
+  </si>
+  <si>
+    <t>HE130005</t>
+  </si>
+  <si>
+    <t>FGWQN</t>
+  </si>
+  <si>
+    <t>5.000.000 ₫</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng Phúc</t>
+  </si>
+  <si>
+    <t>HE130001</t>
+  </si>
+  <si>
+    <t>FPTUHN2</t>
   </si>
   <si>
     <t>Tên bài báo</t>
@@ -65,13 +74,16 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>paper 4</t>
+    <t>paper 7</t>
   </si>
   <si>
     <t>ABC</t>
   </si>
   <si>
-    <t>2 tác giả, 1 địa chỉ FPTU</t>
+    <t>2 tác giả, 2 địa chỉ FPTU</t>
+  </si>
+  <si>
+    <t>paper 8</t>
   </si>
 </sst>
 </file>
@@ -399,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -430,13 +442,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -448,7 +483,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -478,13 +513,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -501,13 +536,36 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -518,7 +576,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -548,6 +606,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -556,7 +631,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
@@ -604,6 +679,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[add] quan ly chuc danh
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Paper.xlsx
+++ b/MANAGER/Excel_template/Download/Paper.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>STT</t>
   </si>
@@ -44,27 +44,6 @@
     <t>Số tiền</t>
   </si>
   <si>
-    <t>Kieu Quoc Tuan</t>
-  </si>
-  <si>
-    <t>HE130005</t>
-  </si>
-  <si>
-    <t>FGWQN</t>
-  </si>
-  <si>
-    <t>5.000.000 ₫</t>
-  </si>
-  <si>
-    <t>Nguyễn Hồng Phúc</t>
-  </si>
-  <si>
-    <t>HE130001</t>
-  </si>
-  <si>
-    <t>FPTUHN2</t>
-  </si>
-  <si>
     <t>Tên bài báo</t>
   </si>
   <si>
@@ -72,18 +51,6 @@
   </si>
   <si>
     <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>paper 7</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>2 tác giả, 2 địa chỉ FPTU</t>
-  </si>
-  <si>
-    <t>paper 8</t>
   </si>
 </sst>
 </file>
@@ -411,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -442,36 +409,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -483,7 +427,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -513,59 +457,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +474,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -606,23 +504,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -631,7 +512,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
@@ -662,40 +543,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[fix] them link cmnd
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/Download/Paper.xlsx
+++ b/MANAGER/Excel_template/Download/Paper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ky 9\Capstone\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieum\Desktop\FPT_Science\MANAGER\Excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -44,6 +44,24 @@
     <t>Số tiền</t>
   </si>
   <si>
+    <t>CMND</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng Phúc</t>
+  </si>
+  <si>
+    <t>HE130001</t>
+  </si>
+  <si>
+    <t>FPTUHN2</t>
+  </si>
+  <si>
+    <t>5.000.000 ₫</t>
+  </si>
+  <si>
+    <t>https://www.google.com.vn/?hl=vi</t>
+  </si>
+  <si>
     <t>Tên bài báo</t>
   </si>
   <si>
@@ -51,6 +69,15 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>paper 9</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>2 tác giả, 2 địa chỉ FPTU</t>
   </si>
 </sst>
 </file>
@@ -409,13 +436,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -427,7 +454,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -457,13 +484,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -474,10 +524,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +553,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -512,10 +565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,9 +595,33 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>